<commit_message>
update run poco on editor
</commit_message>
<xml_diff>
--- a/config/testcases/Report_EEIW01Multisensory(Clone).xlsx
+++ b/config/testcases/Report_EEIW01Multisensory(Clone).xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="198">
   <si>
     <t>TCID</t>
   </si>
@@ -316,10 +316,10 @@
     <t>chuyển trang 2 từ 1</t>
   </si>
   <si>
-    <t>swipe_poco</t>
+    <t>drag_simulate</t>
   </si>
   <si>
-    <t>400,700,300</t>
+    <t>Guiding,0,PointGuiding,0</t>
   </si>
   <si>
     <t>Kiểm tra audio trang 2 từ 1</t>
@@ -332,12 +332,6 @@
   </si>
   <si>
     <t>Chuyển trang 3 từ 1</t>
-  </si>
-  <si>
-    <t>drag_simulate</t>
-  </si>
-  <si>
-    <t>Guiding,0,PointGuiding,0</t>
   </si>
   <si>
     <t>Kiểm tra audio trang 3 từ 1</t>
@@ -2712,10 +2706,10 @@
         <v>103</v>
       </c>
       <c r="D15" s="44" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E15" s="45" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F15" s="41"/>
       <c r="G15" s="37" t="s">
@@ -2749,7 +2743,7 @@
         <v>66</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D16" s="35"/>
       <c r="E16" s="19"/>
@@ -2791,7 +2785,7 @@
         <v>71</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D17" s="41"/>
       <c r="E17" s="47"/>
@@ -2800,16 +2794,16 @@
         <v>13</v>
       </c>
       <c r="H17" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="I17" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="J17" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="I17" s="45" t="s">
-        <v>109</v>
-      </c>
-      <c r="J17" s="48" t="s">
-        <v>110</v>
-      </c>
       <c r="K17" s="48" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L17" s="41"/>
       <c r="M17" s="41"/>
@@ -2835,7 +2829,7 @@
         <v>82</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D18" s="41"/>
       <c r="E18" s="47"/>
@@ -2844,10 +2838,10 @@
         <v>13</v>
       </c>
       <c r="H18" s="44" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I18" s="45" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J18" s="48" t="s">
         <v>92</v>
@@ -2879,13 +2873,13 @@
         <v>62</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D19" s="44" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E19" s="45" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F19" s="41"/>
       <c r="G19" s="37" t="s">
@@ -2919,7 +2913,7 @@
         <v>66</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D20" s="35"/>
       <c r="E20" s="19"/>
@@ -2935,7 +2929,7 @@
       </c>
       <c r="J20" s="41"/>
       <c r="K20" s="36" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L20" s="41"/>
       <c r="M20" s="41"/>
@@ -2961,7 +2955,7 @@
         <v>71</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D21" s="41"/>
       <c r="E21" s="47"/>
@@ -2970,16 +2964,16 @@
         <v>13</v>
       </c>
       <c r="H21" s="44" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I21" s="45" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J21" s="48" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="K21" s="48" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L21" s="41"/>
       <c r="M21" s="41"/>
@@ -3005,7 +2999,7 @@
         <v>82</v>
       </c>
       <c r="C22" s="34" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D22" s="41"/>
       <c r="E22" s="47"/>
@@ -3014,16 +3008,16 @@
         <v>13</v>
       </c>
       <c r="H22" s="44" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I22" s="45" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J22" s="48" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="K22" s="48" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="L22" s="41"/>
       <c r="M22" s="41"/>
@@ -3046,16 +3040,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="34" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C23" s="34" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D23" s="44" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E23" s="45" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F23" s="41"/>
       <c r="G23" s="37" t="s">
@@ -3089,13 +3083,13 @@
         <v>62</v>
       </c>
       <c r="C24" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="D24" s="50" t="s">
+        <v>123</v>
+      </c>
+      <c r="E24" s="51" t="s">
         <v>124</v>
-      </c>
-      <c r="D24" s="50" t="s">
-        <v>125</v>
-      </c>
-      <c r="E24" s="51" t="s">
-        <v>126</v>
       </c>
       <c r="F24" s="36"/>
       <c r="G24" s="37" t="s">
@@ -3109,7 +3103,7 @@
       </c>
       <c r="J24" s="40"/>
       <c r="K24" s="36" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L24" s="41"/>
       <c r="M24" s="41"/>
@@ -3135,7 +3129,7 @@
         <v>66</v>
       </c>
       <c r="C25" s="34" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D25" s="34"/>
       <c r="E25" s="52"/>
@@ -3151,7 +3145,7 @@
       </c>
       <c r="J25" s="40"/>
       <c r="K25" s="46" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="L25" s="41"/>
       <c r="M25" s="41"/>
@@ -3177,7 +3171,7 @@
         <v>71</v>
       </c>
       <c r="C26" s="34" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D26" s="41"/>
       <c r="E26" s="47"/>
@@ -3193,7 +3187,7 @@
       </c>
       <c r="J26" s="41"/>
       <c r="K26" s="48" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L26" s="41"/>
       <c r="M26" s="41"/>
@@ -3219,13 +3213,13 @@
         <v>62</v>
       </c>
       <c r="C27" s="34" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D27" s="44" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E27" s="45" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F27" s="41"/>
       <c r="G27" s="37" t="s">
@@ -3259,7 +3253,7 @@
         <v>66</v>
       </c>
       <c r="C28" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D28" s="35"/>
       <c r="E28" s="19"/>
@@ -3275,7 +3269,7 @@
       </c>
       <c r="J28" s="40"/>
       <c r="K28" s="36" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L28" s="41"/>
       <c r="M28" s="41"/>
@@ -3301,7 +3295,7 @@
         <v>71</v>
       </c>
       <c r="C29" s="34" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D29" s="41"/>
       <c r="E29" s="47"/>
@@ -3317,7 +3311,7 @@
       </c>
       <c r="J29" s="41"/>
       <c r="K29" s="48" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L29" s="41"/>
       <c r="M29" s="41"/>
@@ -3343,13 +3337,13 @@
         <v>62</v>
       </c>
       <c r="C30" s="34" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D30" s="44" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E30" s="45" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F30" s="41"/>
       <c r="G30" s="37" t="s">
@@ -3383,7 +3377,7 @@
         <v>66</v>
       </c>
       <c r="C31" s="34" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D31" s="35"/>
       <c r="E31" s="19"/>
@@ -3399,7 +3393,7 @@
       </c>
       <c r="J31" s="40"/>
       <c r="K31" s="36" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L31" s="41"/>
       <c r="M31" s="41"/>
@@ -3425,7 +3419,7 @@
         <v>71</v>
       </c>
       <c r="C32" s="34" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D32" s="41"/>
       <c r="E32" s="47"/>
@@ -3434,16 +3428,16 @@
         <v>13</v>
       </c>
       <c r="H32" s="44" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I32" s="45" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J32" s="48" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K32" s="48" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="L32" s="41"/>
       <c r="M32" s="41"/>
@@ -3469,7 +3463,7 @@
         <v>82</v>
       </c>
       <c r="C33" s="34" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D33" s="41"/>
       <c r="E33" s="47"/>
@@ -3478,16 +3472,16 @@
         <v>13</v>
       </c>
       <c r="H33" s="44" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I33" s="45" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J33" s="48" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="K33" s="48" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="L33" s="41"/>
       <c r="M33" s="41"/>
@@ -3513,13 +3507,13 @@
         <v>62</v>
       </c>
       <c r="C34" s="34" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D34" s="44" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E34" s="45" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F34" s="41"/>
       <c r="G34" s="37" t="s">
@@ -3553,7 +3547,7 @@
         <v>66</v>
       </c>
       <c r="C35" s="34" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D35" s="35"/>
       <c r="E35" s="19"/>
@@ -3569,7 +3563,7 @@
       </c>
       <c r="J35" s="41"/>
       <c r="K35" s="36" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="L35" s="41"/>
       <c r="M35" s="41"/>
@@ -3595,7 +3589,7 @@
         <v>71</v>
       </c>
       <c r="C36" s="34" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D36" s="41"/>
       <c r="E36" s="47"/>
@@ -3604,16 +3598,16 @@
         <v>13</v>
       </c>
       <c r="H36" s="44" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I36" s="45" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J36" s="48" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K36" s="48" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="L36" s="41"/>
       <c r="M36" s="41"/>
@@ -3639,7 +3633,7 @@
         <v>82</v>
       </c>
       <c r="C37" s="34" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D37" s="41"/>
       <c r="E37" s="47"/>
@@ -3648,16 +3642,16 @@
         <v>13</v>
       </c>
       <c r="H37" s="44" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I37" s="45" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J37" s="48" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K37" s="48" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="L37" s="41"/>
       <c r="M37" s="41"/>
@@ -3680,16 +3674,16 @@
         <v>30</v>
       </c>
       <c r="B38" s="53" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C38" s="53" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D38" s="44" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E38" s="45" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F38" s="54"/>
       <c r="G38" s="55" t="s">
@@ -3723,13 +3717,13 @@
         <v>62</v>
       </c>
       <c r="C39" s="53" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D39" s="50" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E39" s="51" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F39" s="39"/>
       <c r="G39" s="55" t="s">
@@ -3743,7 +3737,7 @@
       </c>
       <c r="J39" s="22"/>
       <c r="K39" s="56" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="L39" s="21"/>
       <c r="M39" s="21"/>
@@ -3769,7 +3763,7 @@
         <v>66</v>
       </c>
       <c r="C40" s="53" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D40" s="34"/>
       <c r="E40" s="52"/>
@@ -3785,7 +3779,7 @@
       </c>
       <c r="J40" s="21"/>
       <c r="K40" s="46" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L40" s="21"/>
       <c r="M40" s="21"/>
@@ -3811,7 +3805,7 @@
         <v>71</v>
       </c>
       <c r="C41" s="53" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D41" s="41"/>
       <c r="E41" s="47"/>
@@ -3827,7 +3821,7 @@
       </c>
       <c r="J41" s="22"/>
       <c r="K41" s="57" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L41" s="21"/>
       <c r="M41" s="21"/>
@@ -3853,13 +3847,13 @@
         <v>62</v>
       </c>
       <c r="C42" s="53" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D42" s="44" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E42" s="45" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F42" s="54"/>
       <c r="G42" s="55" t="s">
@@ -3893,7 +3887,7 @@
         <v>66</v>
       </c>
       <c r="C43" s="53" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D43" s="58"/>
       <c r="E43" s="19"/>
@@ -3909,7 +3903,7 @@
       </c>
       <c r="J43" s="21"/>
       <c r="K43" s="56" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="L43" s="21"/>
       <c r="M43" s="21"/>
@@ -3935,7 +3929,7 @@
         <v>71</v>
       </c>
       <c r="C44" s="53" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D44" s="41"/>
       <c r="E44" s="47"/>
@@ -3951,7 +3945,7 @@
       </c>
       <c r="J44" s="22"/>
       <c r="K44" s="57" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L44" s="21"/>
       <c r="M44" s="21"/>
@@ -3977,13 +3971,13 @@
         <v>62</v>
       </c>
       <c r="C45" s="53" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D45" s="44" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E45" s="45" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F45" s="54"/>
       <c r="G45" s="55" t="s">
@@ -4017,7 +4011,7 @@
         <v>66</v>
       </c>
       <c r="C46" s="53" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D46" s="58"/>
       <c r="E46" s="19"/>
@@ -4033,7 +4027,7 @@
       </c>
       <c r="J46" s="40"/>
       <c r="K46" s="56" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="L46" s="21"/>
       <c r="M46" s="21"/>
@@ -4059,7 +4053,7 @@
         <v>71</v>
       </c>
       <c r="C47" s="53" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D47" s="21"/>
       <c r="E47" s="19"/>
@@ -4068,16 +4062,16 @@
         <v>13</v>
       </c>
       <c r="H47" s="38" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I47" s="39" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J47" s="46" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K47" s="46" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L47" s="21"/>
       <c r="M47" s="21"/>
@@ -4103,7 +4097,7 @@
         <v>82</v>
       </c>
       <c r="C48" s="53" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D48" s="41"/>
       <c r="E48" s="47"/>
@@ -4112,16 +4106,16 @@
         <v>13</v>
       </c>
       <c r="H48" s="38" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I48" s="39" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J48" s="38" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="K48" s="57" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L48" s="21"/>
       <c r="M48" s="21"/>
@@ -4147,13 +4141,13 @@
         <v>62</v>
       </c>
       <c r="C49" s="53" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D49" s="44" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E49" s="45" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F49" s="54"/>
       <c r="G49" s="55" t="s">
@@ -4187,7 +4181,7 @@
         <v>66</v>
       </c>
       <c r="C50" s="53" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D50" s="58"/>
       <c r="E50" s="19"/>
@@ -4203,7 +4197,7 @@
       </c>
       <c r="J50" s="40"/>
       <c r="K50" s="56" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="L50" s="21"/>
       <c r="M50" s="21"/>
@@ -4229,7 +4223,7 @@
         <v>71</v>
       </c>
       <c r="C51" s="53" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D51" s="21"/>
       <c r="E51" s="19"/>
@@ -4238,16 +4232,16 @@
         <v>13</v>
       </c>
       <c r="H51" s="38" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I51" s="39" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J51" s="46" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="K51" s="46" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="L51" s="21"/>
       <c r="M51" s="21"/>
@@ -4273,7 +4267,7 @@
         <v>82</v>
       </c>
       <c r="C52" s="53" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D52" s="41"/>
       <c r="E52" s="47"/>
@@ -4282,16 +4276,16 @@
         <v>13</v>
       </c>
       <c r="H52" s="38" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I52" s="39" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J52" s="57" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K52" s="57" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="L52" s="21"/>
       <c r="M52" s="21"/>
@@ -4314,16 +4308,16 @@
         <v>38</v>
       </c>
       <c r="B53" s="53" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C53" s="53" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D53" s="44" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E53" s="45" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F53" s="54"/>
       <c r="G53" s="55" t="s">
@@ -4357,13 +4351,13 @@
         <v>62</v>
       </c>
       <c r="C54" s="53" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D54" s="50" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E54" s="51" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F54" s="39"/>
       <c r="G54" s="55" t="s">
@@ -4377,7 +4371,7 @@
       </c>
       <c r="J54" s="22"/>
       <c r="K54" s="56" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="L54" s="21"/>
       <c r="M54" s="21"/>
@@ -4403,7 +4397,7 @@
         <v>66</v>
       </c>
       <c r="C55" s="53" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D55" s="34"/>
       <c r="E55" s="52"/>
@@ -4419,7 +4413,7 @@
       </c>
       <c r="J55" s="21"/>
       <c r="K55" s="46" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="L55" s="21"/>
       <c r="M55" s="21"/>
@@ -4445,7 +4439,7 @@
         <v>71</v>
       </c>
       <c r="C56" s="53" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D56" s="41"/>
       <c r="E56" s="47"/>
@@ -4461,7 +4455,7 @@
       </c>
       <c r="J56" s="22"/>
       <c r="K56" s="57" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="L56" s="21"/>
       <c r="M56" s="21"/>
@@ -4487,13 +4481,13 @@
         <v>62</v>
       </c>
       <c r="C57" s="53" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D57" s="44" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E57" s="45" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F57" s="54"/>
       <c r="G57" s="55" t="s">
@@ -4527,7 +4521,7 @@
         <v>66</v>
       </c>
       <c r="C58" s="53" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D58" s="58"/>
       <c r="E58" s="19"/>
@@ -4543,7 +4537,7 @@
       </c>
       <c r="J58" s="21"/>
       <c r="K58" s="56" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="L58" s="21"/>
       <c r="M58" s="21"/>
@@ -4569,7 +4563,7 @@
         <v>71</v>
       </c>
       <c r="C59" s="53" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D59" s="21"/>
       <c r="E59" s="19"/>
@@ -4585,7 +4579,7 @@
       </c>
       <c r="J59" s="21"/>
       <c r="K59" s="46" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="L59" s="21"/>
       <c r="M59" s="21"/>
@@ -4611,13 +4605,13 @@
         <v>62</v>
       </c>
       <c r="C60" s="53" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D60" s="44" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E60" s="45" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F60" s="21"/>
       <c r="G60" s="55" t="s">
@@ -4651,7 +4645,7 @@
         <v>66</v>
       </c>
       <c r="C61" s="53" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D61" s="58"/>
       <c r="E61" s="19"/>
@@ -4667,7 +4661,7 @@
       </c>
       <c r="J61" s="21"/>
       <c r="K61" s="56" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="L61" s="21"/>
       <c r="M61" s="21"/>
@@ -4693,7 +4687,7 @@
         <v>71</v>
       </c>
       <c r="C62" s="53" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D62" s="21"/>
       <c r="E62" s="19"/>
@@ -4702,16 +4696,16 @@
         <v>13</v>
       </c>
       <c r="H62" s="38" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I62" s="39" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J62" s="38" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K62" s="46" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L62" s="21"/>
       <c r="M62" s="21"/>
@@ -4737,7 +4731,7 @@
         <v>82</v>
       </c>
       <c r="C63" s="53" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D63" s="21"/>
       <c r="E63" s="19"/>
@@ -4746,16 +4740,16 @@
         <v>13</v>
       </c>
       <c r="H63" s="38" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I63" s="39" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J63" s="38" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="K63" s="46" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="L63" s="21"/>
       <c r="M63" s="21"/>
@@ -4781,13 +4775,13 @@
         <v>62</v>
       </c>
       <c r="C64" s="53" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D64" s="44" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E64" s="45" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F64" s="21"/>
       <c r="G64" s="55" t="s">
@@ -4821,7 +4815,7 @@
         <v>66</v>
       </c>
       <c r="C65" s="53" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D65" s="50"/>
       <c r="E65" s="19"/>
@@ -4837,7 +4831,7 @@
       </c>
       <c r="J65" s="22"/>
       <c r="K65" s="60" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="L65" s="21"/>
       <c r="M65" s="21"/>
@@ -4863,7 +4857,7 @@
         <v>71</v>
       </c>
       <c r="C66" s="53" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D66" s="21"/>
       <c r="E66" s="19"/>
@@ -4872,16 +4866,16 @@
         <v>13</v>
       </c>
       <c r="H66" s="38" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I66" s="39" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J66" s="46" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="K66" s="46" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="L66" s="21"/>
       <c r="M66" s="21"/>
@@ -4907,7 +4901,7 @@
         <v>82</v>
       </c>
       <c r="C67" s="53" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D67" s="21"/>
       <c r="E67" s="19"/>
@@ -4916,16 +4910,16 @@
         <v>13</v>
       </c>
       <c r="H67" s="38" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I67" s="39" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J67" s="46" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="K67" s="46" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="L67" s="21"/>
       <c r="M67" s="21"/>
@@ -4948,16 +4942,16 @@
         <v>46</v>
       </c>
       <c r="B68" s="53" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C68" s="53" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D68" s="44" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E68" s="45" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F68" s="21"/>
       <c r="G68" s="55" t="s">
@@ -4991,13 +4985,13 @@
         <v>62</v>
       </c>
       <c r="C69" s="42" t="s">
+        <v>185</v>
+      </c>
+      <c r="D69" s="42" t="s">
+        <v>186</v>
+      </c>
+      <c r="E69" s="31" t="s">
         <v>187</v>
-      </c>
-      <c r="D69" s="42" t="s">
-        <v>188</v>
-      </c>
-      <c r="E69" s="31" t="s">
-        <v>189</v>
       </c>
       <c r="F69" s="19"/>
       <c r="G69" s="61" t="s">
@@ -5031,13 +5025,13 @@
         <v>66</v>
       </c>
       <c r="C70" s="63" t="s">
+        <v>188</v>
+      </c>
+      <c r="D70" s="63" t="s">
+        <v>189</v>
+      </c>
+      <c r="E70" s="19" t="s">
         <v>190</v>
-      </c>
-      <c r="D70" s="63" t="s">
-        <v>191</v>
-      </c>
-      <c r="E70" s="19" t="s">
-        <v>192</v>
       </c>
       <c r="F70" s="64"/>
       <c r="G70" s="65" t="s">
@@ -5077,7 +5071,7 @@
         <v>64</v>
       </c>
       <c r="E71" s="19" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F71" s="19"/>
       <c r="G71" s="20" t="s">
@@ -5111,13 +5105,13 @@
         <v>66</v>
       </c>
       <c r="C72" s="13" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D72" s="13" t="s">
         <v>73</v>
       </c>
       <c r="E72" s="19" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F72" s="19"/>
       <c r="G72" s="20" t="s">
@@ -5260,10 +5254,10 @@
         <v>5</v>
       </c>
       <c r="B1" s="69" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C1" s="69" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -34775,10 +34769,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="66" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B1" s="81" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>